<commit_message>
Add Excel Data Driven RestAssured Test
</commit_message>
<xml_diff>
--- a/restassuredpractice/src/main/resources/xlstest.xlsx
+++ b/restassuredpractice/src/main/resources/xlstest.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="RestAssured" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t xml:space="preserve">Testcases</t>
   </si>
@@ -34,49 +35,37 @@
     <t xml:space="preserve">Data3</t>
   </si>
   <si>
-    <t xml:space="preserve">Login</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Drampa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gothitelle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Actillery</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Purchase</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Flaaffy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Urshifu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Add Profile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Serperior</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lilligant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Decidueye</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Delete Profile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aegislash</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scrafty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Togekiss</t>
+    <t xml:space="preserve">Data4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LibraryAddBook</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Learn Appium Automation with Java</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">John Foe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isbn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aisle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">author</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patchouli Knowledge</t>
   </si>
 </sst>
 </file>
@@ -185,13 +174,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="53.63"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -206,63 +198,31 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="C2" s="0" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="D2" s="0" t="n">
+        <v>999</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="1" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
+    </row>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
@@ -272,4 +232,65 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.79"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>999</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>